<commit_message>
correction non-corpo, inventaire et xlsx
</commit_message>
<xml_diff>
--- a/useCase/tableau USECASE.xlsx
+++ b/useCase/tableau USECASE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Data\Analyse_relationnelle\useCase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Analyse_relationnelle\useCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AD2049-286B-4EB8-87EF-C755EF9D5815}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBA12DA-3FDC-46E6-A9AA-A7292B98EC7A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{E072AD6C-52D8-4966-BF5B-15FDDEF42E98}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E072AD6C-52D8-4966-BF5B-15FDDEF42E98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Passer une commande en tant qu'une compagnie</t>
   </si>
@@ -78,6 +76,24 @@
   </si>
   <si>
     <t>vend divers produits en lot qu’elle achète auprès de plusieurs fournisseurs</t>
+  </si>
+  <si>
+    <t>Acteurs</t>
+  </si>
+  <si>
+    <t>SGP</t>
+  </si>
+  <si>
+    <t>SGC</t>
+  </si>
+  <si>
+    <t>Personne morale</t>
+  </si>
+  <si>
+    <t>Personne physique</t>
+  </si>
+  <si>
+    <t>Client non enregistré</t>
   </si>
 </sst>
 </file>
@@ -109,7 +125,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,19 +134,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF61D6FF"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -162,17 +184,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,85 +517,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DFA237-9047-46E8-A214-282656A57C79}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>